<commit_message>
Updated the file for Algeria
Updated file and download spreadsheet.
</commit_message>
<xml_diff>
--- a/Teams/downloads/country-and-region-availabilty/country-and-region-availability-(v-06242020)-(en-us).xlsx
+++ b/Teams/downloads/country-and-region-availabilty/country-and-region-availability-(v-06242020)-(en-us).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5BD9B6C-DE1B-438D-BDE2-5190D4CF825C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E95BAD2-2F08-475B-BB15-885AFC3D7FD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="2220" windowWidth="21885" windowHeight="12885" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Audio Conferencing purchase" sheetId="1" r:id="rId1"/>
@@ -1988,7 +1988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B106"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
@@ -2854,7 +2854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -3658,7 +3658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A183" sqref="A183"/>
     </sheetView>
   </sheetViews>
@@ -8257,7 +8257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A103"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>

</xml_diff>